<commit_message>
update testing - v.6
</commit_message>
<xml_diff>
--- a/tes_2.xlsx
+++ b/tes_2.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -962,6 +962,561 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>11:37:38</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien filter en palet</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11:45:06</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Tornillo atascado en tolva</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11:47:46</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>11:52:36</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>11:52:39</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Fallo visión core</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11:52:45</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11:52:50</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Secuencia atornillador</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:52:55</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Colisión placas</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:53:03</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:53:06</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>11:53:35</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Tornillo atascado en tolva</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>11:53:39</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Top cover</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>11:55:00</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>11:55:04</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Tornillo atascado</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>11:55:07</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Colisión placas</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel view perfect update / new graph interface v.7
</commit_message>
<xml_diff>
--- a/tes_2.xlsx
+++ b/tes_2.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -410,37 +410,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>2024-05-13</t>
+          <t>Fecha</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>11:06:09</t>
+          <t>Hora</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>WC47 NACP</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>WC48 P5F</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>WC49 P5H</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>WV50 FILTER</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Colisión placas</t>
+          <t>SPL</t>
         </is>
       </c>
     </row>
@@ -1514,6 +1514,1449 @@
       <c r="G30" t="inlineStr">
         <is>
           <t>Colisión placas</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>11:59:57</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Atasco tuerca</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>12:05:10</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>12:05:14</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Atasco tuerca</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>12:05:18</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien ferrita</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>12:06:45</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>12:13:21</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Robot no coge PCB</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>12:13:27</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>12:22:33</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Robot no coge PCB</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>12:22:36</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Marco atascado en parte inferior</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>12:25:17</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Fallo etiqueta</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>12:25:27</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>12:25:57</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>No detecta presencia power CP</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>12:26:01</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>No coloca bien la pcb</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>12:26:05</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Error en sensor de salida</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>12:26:27</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Power CP</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>12:26:30</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>No coloca bien el sealling</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>12:26:34</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Fallo visión core</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>12:29:16</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>12:29:19</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>12:29:22</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Top cover</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>12:29:27</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>No lee QR</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>12:29:32</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Error en sensor de salida</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>12:29:39</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>12:29:41</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>12:29:43</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>12:32:27</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Secuencia atornillador</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>12:32:32</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Fallo fijador tapa</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>12:32:34</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Fallo fijador tapa</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>12:32:38</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Marco atascado en parte inferior</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>12:36:50</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Fallo tolva</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>12:36:56</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>12:37:05</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>12:37:09</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Core enganchado</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>12:37:21</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Secuencia atornillador</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>12:37:24</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien ferrita</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>12:37:37</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>12:38:08</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>No detecta presencia power CP</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>12:38:17</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Cámara no detecta busbar</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
graph update - v.7.1
</commit_message>
<xml_diff>
--- a/tes_2.xlsx
+++ b/tes_2.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -2960,6 +2960,80 @@
         </is>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>12:44:57</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>12:45:02</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Tornillo atascado en tolva</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
config test 2 and 3 - v.7.5
</commit_message>
<xml_diff>
--- a/tes_2.xlsx
+++ b/tes_2.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -3034,6 +3034,1597 @@
         </is>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>14:58:17</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>14:58:19</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>14:58:22</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Fallo cámara visión</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>14:58:29</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>15:05:16</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Secuencia atornillador</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>15:09:22</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Secuencia atornillador</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>15:50:56</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>15:51:00</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foam derecho</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>15:51:03</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>15:51:07</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Core enganchado</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>15:51:13</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Cover atascado</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>15:54:01</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Power CP</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>15:56:55</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>15:56:59</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>15:57:06</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>No coloca bien el sealling</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>15:57:19</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>16:00:23</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>16:00:30</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>16:00:32</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>16:02:12</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>AOI no detecta pieza</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>16:02:16</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>16:02:29</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>16:02:37</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>No coloca bien el sealling</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>16:03:20</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Cámara no detecta busbar</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>16:08:27</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>16:08:30</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>16:08:40</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>16:08:46</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>16:09:02</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>No detecta presencia power CP</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>16:09:12</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>No detecta presencia power CP</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>16:10:16</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>16:10:27</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Atasco tuerca</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>16:11:52</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>16:12:00</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>16:12:07</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>16:31:07</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>16:31:11</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>16:31:29</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>16:31:34</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>No detecta presencia power CP</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>16:31:38</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>16:31:49</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Fallo tolva</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>16:31:51</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Fallo cámara visión</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new logo - sign in / v.7.7 / testing.py
</commit_message>
<xml_diff>
--- a/tes_2.xlsx
+++ b/tes_2.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:G127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -4625,6 +4625,487 @@
         </is>
       </c>
     </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>09:30:16</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>09:30:23</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>AOI no detecta pieza</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>09:30:31</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>09:30:38</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Fallo cámara visión</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>09:30:44</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>09:30:53</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>No coloca bien la pcb</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>09:30:56</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Fallo cámara cover</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>09:34:15</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>09:51:40</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Secuencia atornillador</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>09:56:09</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>09:56:59</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>Fallo visión core</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>09:57:04</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Repeat funcional</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>09:57:08</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Fallo cámara ferrite</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update testing.py / v.7.8
</commit_message>
<xml_diff>
--- a/tes_2.xlsx
+++ b/tes_2.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G127"/>
+  <dimension ref="A1:G129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -5106,6 +5106,80 @@
         </is>
       </c>
     </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>10:29:43</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>10:33:57</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Power CP</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new filter / testing_copy_filter.py / v.8.0
</commit_message>
<xml_diff>
--- a/tes_2.xlsx
+++ b/tes_2.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G158"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -5180,6 +5180,1079 @@
         </is>
       </c>
     </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>11:20:09</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>11:20:16</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>AOI no detecta pieza</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>11:20:27</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>11:22:33</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Secuencia atornillador</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>11:26:32</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>11:26:50</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Pieza enganchada en HV Test</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>11:26:53</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Core enganchado</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>11:26:56</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>11:26:59</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Fallo cámara QR</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>11:30:59</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>11:35:13</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Tornillo atascado en tolva</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>11:35:17</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>No lee QR</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>11:35:32</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>11:35:37</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien filter en palet</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>11:35:43</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Core enganchado</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>11:39:49</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>11:42:40</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Secuencia atornillador</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>11:43:49</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Robot no coge PCB</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>11:43:55</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Cover atascado</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>11:45:47</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>11:47:03</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>11:58:11</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>12:09:25</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>12:16:33</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>12:16:37</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>12:16:48</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Repeat funcional</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>12:16:52</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Core enganchado</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>12:16:57</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien filter en palet</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>12:17:01</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating filter / testing_copy_filter.py / v.8.5
</commit_message>
<xml_diff>
--- a/tes_2.xlsx
+++ b/tes_2.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G158"/>
+  <dimension ref="A1:G159"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -6253,6 +6253,43 @@
         </is>
       </c>
     </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>12:23:12</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foam derecho</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
filter finished / testing_copy_filter.py / v.8.8
</commit_message>
<xml_diff>
--- a/tes_2.xlsx
+++ b/tes_2.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G159"/>
+  <dimension ref="A1:G164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -6290,6 +6290,191 @@
         </is>
       </c>
     </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>12:30:16</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Fallo fijador tapa</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>12:30:23</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>No detecta presencia power CP</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>12:34:20</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>12:34:24</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>12:34:28</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Fallo fijador tapa</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new tickets / tes_2.xlsx
</commit_message>
<xml_diff>
--- a/tes_2.xlsx
+++ b/tes_2.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G164"/>
+  <dimension ref="A1:G165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -6475,6 +6475,43 @@
         </is>
       </c>
     </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>12:46:15</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update filter / more filters / update testing_copy_filter / v.9.0
</commit_message>
<xml_diff>
--- a/tes_2.xlsx
+++ b/tes_2.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G167"/>
+  <dimension ref="A1:G170"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -6586,6 +6586,117 @@
         </is>
       </c>
     </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>18:25:34</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>18:25:42</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>18:31:21</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Power CP</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating filters / testing_copy_filter.py / v.9.5
</commit_message>
<xml_diff>
--- a/tes_2.xlsx
+++ b/tes_2.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G170"/>
+  <dimension ref="A1:G174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -6697,6 +6697,154 @@
         </is>
       </c>
     </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>18:56:57</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Tornillo atascado en tolva</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>18:57:01</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Fallo etiqueta</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>19:23:33</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>19:31:47</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>Atasco tuerca</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>